<commit_message>
added validation functions and converted the project for automating facebook
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
   <si>
     <t>a1</t>
   </si>
@@ -82,6 +82,12 @@
   </si>
   <si>
     <t>LoginTest</t>
+  </si>
+  <si>
+    <t>vaibhavcool20@protonmail.com</t>
+  </si>
+  <si>
+    <t>xxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -436,8 +442,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="9.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -461,15 +467,15 @@
         <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>0</v>
+        <v>19</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
added several pages and created a new profile test
</commit_message>
<xml_diff>
--- a/Data.xlsx
+++ b/Data.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="19">
   <si>
     <t>a1</t>
   </si>
@@ -51,24 +51,9 @@
     <t>a6</t>
   </si>
   <si>
-    <t>TestB</t>
-  </si>
-  <si>
     <t>TestC</t>
   </si>
   <si>
-    <t>Col3</t>
-  </si>
-  <si>
-    <t>Col4</t>
-  </si>
-  <si>
-    <t>Col5</t>
-  </si>
-  <si>
-    <t>Col6</t>
-  </si>
-  <si>
     <t>Runmode</t>
   </si>
   <si>
@@ -87,7 +72,16 @@
     <t>vaibhavcool20@protonmail.com</t>
   </si>
   <si>
-    <t>xxxxxxx</t>
+    <t>ProfileTest</t>
+  </si>
+  <si>
+    <t>ProfileName</t>
+  </si>
+  <si>
+    <t>Vaibhav Gupta</t>
+  </si>
+  <si>
+    <t>xxxxxxxx</t>
   </si>
 </sst>
 </file>
@@ -434,26 +428,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="30.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>3</v>
@@ -464,18 +459,18 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
         <v>2</v>
@@ -486,7 +481,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -497,12 +492,12 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>3</v>
@@ -511,156 +506,72 @@
         <v>4</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="G8" s="2" t="s">
-        <v>13</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
       <c r="B9" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>18</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
         <v>0</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>1</v>
       </c>
-      <c r="D9" t="s">
-        <v>0</v>
-      </c>
-      <c r="E9" t="s">
-        <v>1</v>
-      </c>
-      <c r="F9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>15</v>
-      </c>
-      <c r="B10" t="s">
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>10</v>
+      </c>
+      <c r="B14" t="s">
         <v>2</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C14" t="s">
         <v>5</v>
       </c>
-      <c r="D10" t="s">
-        <v>2</v>
-      </c>
-      <c r="E10" t="s">
-        <v>5</v>
-      </c>
-      <c r="F10" t="s">
-        <v>5</v>
-      </c>
-      <c r="G10" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>15</v>
-      </c>
-      <c r="B11" t="s">
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" t="s">
         <v>6</v>
       </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-      <c r="D11" t="s">
-        <v>6</v>
-      </c>
-      <c r="E11" t="s">
-        <v>7</v>
-      </c>
-      <c r="F11" t="s">
-        <v>7</v>
-      </c>
-      <c r="G11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B12" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-      <c r="D12" t="s">
-        <v>6</v>
-      </c>
-      <c r="E12" t="s">
-        <v>7</v>
-      </c>
-      <c r="F12" t="s">
-        <v>7</v>
-      </c>
-      <c r="G12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="C15" s="2" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B16" t="s">
-        <v>0</v>
-      </c>
-      <c r="C16" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>15</v>
-      </c>
-      <c r="B18" t="s">
-        <v>6</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="C15" t="s">
         <v>7</v>
       </c>
     </row>
@@ -673,7 +584,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -683,34 +596,34 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>17</v>
+        <v>12</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>14</v>
+        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>18</v>
+        <v>13</v>
       </c>
       <c r="B2" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>8</v>
+        <v>15</v>
       </c>
       <c r="B3" t="s">
-        <v>15</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>